<commit_message>
Add 'Check Downloaded Excel File' test
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Vacancy.xlsx
+++ b/cypress/fixtures/Vacancy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\Full stack course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\QA\Automation\Tasks\GSG - Cypress\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{222CD81E-3FC2-4021-8205-E98AE2DB3B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9E43EE-86D9-421C-A009-62176D2BFFF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{554F4615-CC65-4C0F-851F-EE37090823D3}"/>
+    <workbookView xWindow="4944" yWindow="3276" windowWidth="17280" windowHeight="8964" xr2:uid="{554F4615-CC65-4C0F-851F-EE37090823D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <t>Hakoona Matata</t>
   </si>
   <si>
-    <t>Nablus</t>
+    <t>Spacetoon</t>
   </si>
 </sst>
 </file>
@@ -429,12 +429,13 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -453,7 +454,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="2">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>4</v>

</xml_diff>